<commit_message>
working on reading in TripAndLeaderStatusInfo
</commit_message>
<xml_diff>
--- a/Example_Data/TripsAndLeaderStatusInfo.xlsx
+++ b/Example_Data/TripsAndLeaderStatusInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lduli\TripPrefVisualizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shume\Documents\Example Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14B149-6742-4859-83D5-E598D3591C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BDDDA9-A245-4A5F-B8EA-72107B14CDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
+    <workbookView xWindow="20" yWindow="720" windowWidth="23980" windowHeight="15280" activeTab="1" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefs Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
   <si>
     <t>Start Date</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Total LG</t>
+  </si>
+  <si>
+    <t>UF ID</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -863,11 +866,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,6 +1062,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56457AC2-4CCE-48AB-B957-6565BDA2DBE4}">
   <dimension ref="B2:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1413,11 +1449,11 @@
       </c>
       <c r="H3" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1, 6), "Overnight", "Biking","Spelunking", "Watersports", "Surfing", "Sea Kayaking")</f>
-        <v>Watersports</v>
+        <v>Biking</v>
       </c>
       <c r="J3">
         <f ca="1">CHOOSE(RANDBETWEEN(1, 2), 2, 4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2551,545 +2587,587 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445B6131-D158-4A66-8748-C0EBB6C75469}">
-  <dimension ref="B3:L35"/>
+  <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" customWidth="1"/>
-    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="72" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="73"/>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="73"/>
+      <c r="E3" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="73"/>
       <c r="F3" s="73"/>
       <c r="G3" s="73"/>
       <c r="H3" s="73"/>
       <c r="I3" s="73"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="35"/>
       <c r="L3" s="35"/>
-    </row>
-    <row r="4" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M3" s="35"/>
+    </row>
+    <row r="4" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="D4" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="F4" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="G4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="I4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="J4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="35"/>
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
-    </row>
-    <row r="5" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M4" s="35"/>
+    </row>
+    <row r="5" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B5" s="41">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="77">
         <v>2020</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="D5" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="E5" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="F5" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="43" t="s">
-        <v>75</v>
-      </c>
+      <c r="G5" s="44"/>
       <c r="H5" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="45"/>
-      <c r="J5" s="35"/>
+      <c r="I5" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="45"/>
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
-    </row>
-    <row r="6" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M5" s="35"/>
+    </row>
+    <row r="6" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B6" s="46">
+        <v>12345679</v>
+      </c>
+      <c r="C6" s="78">
         <v>2020</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="D6" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="E6" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="49"/>
       <c r="F6" s="49"/>
-      <c r="G6" s="50" t="s">
-        <v>75</v>
-      </c>
+      <c r="G6" s="49"/>
       <c r="H6" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="35"/>
+      <c r="J6" s="51" t="s">
+        <v>75</v>
+      </c>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
-    </row>
-    <row r="7" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B7" s="46">
+        <v>12456781</v>
+      </c>
+      <c r="C7" s="78">
         <v>2021</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="D7" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="E7" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="49"/>
+      <c r="G7" s="52" t="s">
         <v>78</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>75</v>
       </c>
       <c r="H7" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="I7" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="35"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
-    </row>
-    <row r="8" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
       <c r="H8" s="49"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="35"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="68"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-    </row>
-    <row r="9" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M8" s="35"/>
+    </row>
+    <row r="9" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="49"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
       <c r="H9" s="49"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="74" t="s">
+      <c r="I9" s="49"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="75"/>
-    </row>
-    <row r="10" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M9" s="75"/>
+    </row>
+    <row r="10" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="49"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="67"/>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
       <c r="H10" s="49"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="54" t="s">
+      <c r="I10" s="49"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="55" t="s">
+      <c r="M10" s="55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="49"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
       <c r="H11" s="49"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="57" t="s">
+      <c r="I11" s="49"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="L11" s="56" t="s">
+      <c r="M11" s="56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="49"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="66" t="s">
+      <c r="I12" s="49"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="49"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="63"/>
-    </row>
-    <row r="14" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="I13" s="49"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="63"/>
+    </row>
+    <row r="14" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="49"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="49"/>
       <c r="G14" s="49"/>
       <c r="H14" s="49"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="63"/>
-    </row>
-    <row r="15" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="I14" s="49"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="63"/>
+    </row>
+    <row r="15" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="49"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="49"/>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="35"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
-    </row>
-    <row r="16" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M15" s="35"/>
+    </row>
+    <row r="16" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="49"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="49"/>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35"/>
-    </row>
-    <row r="17" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="49"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="49"/>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="35"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="68"/>
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
-    </row>
-    <row r="18" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="49"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="49"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="35"/>
-    </row>
-    <row r="19" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="I18" s="49"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="35"/>
+    </row>
+    <row r="19" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="49"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="49"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="35"/>
-    </row>
-    <row r="20" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="I19" s="49"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="35"/>
+    </row>
+    <row r="20" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="49"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="35"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="35"/>
       <c r="L20" s="35"/>
-    </row>
-    <row r="21" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M20" s="35"/>
+    </row>
+    <row r="21" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="49"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="35"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="68"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
-    </row>
-    <row r="22" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M21" s="35"/>
+    </row>
+    <row r="22" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="49"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="35"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="68"/>
       <c r="K22" s="35"/>
       <c r="L22" s="35"/>
-    </row>
-    <row r="23" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M22" s="35"/>
+    </row>
+    <row r="23" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B23" s="46"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="49"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="35"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="68"/>
       <c r="K23" s="35"/>
       <c r="L23" s="35"/>
-    </row>
-    <row r="24" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M23" s="35"/>
+    </row>
+    <row r="24" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="49"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="67"/>
       <c r="F24" s="49"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="35"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="68"/>
       <c r="K24" s="35"/>
       <c r="L24" s="35"/>
-    </row>
-    <row r="25" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M24" s="35"/>
+    </row>
+    <row r="25" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B25" s="46"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="49"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="49"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="35"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="68"/>
       <c r="K25" s="35"/>
       <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M25" s="35"/>
+    </row>
+    <row r="26" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="49"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="67"/>
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="35"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="68"/>
       <c r="K26" s="35"/>
       <c r="L26" s="35"/>
-    </row>
-    <row r="27" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M26" s="35"/>
+    </row>
+    <row r="27" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B27" s="46"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="49"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="49"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="35"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="68"/>
       <c r="K27" s="35"/>
       <c r="L27" s="35"/>
-    </row>
-    <row r="28" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M27" s="35"/>
+    </row>
+    <row r="28" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="49"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="67"/>
       <c r="F28" s="49"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="35"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="68"/>
       <c r="K28" s="35"/>
       <c r="L28" s="35"/>
-    </row>
-    <row r="29" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M28" s="35"/>
+    </row>
+    <row r="29" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B29" s="46"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="49"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="67"/>
       <c r="F29" s="49"/>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="35"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="68"/>
       <c r="K29" s="35"/>
       <c r="L29" s="35"/>
-    </row>
-    <row r="30" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M29" s="35"/>
+    </row>
+    <row r="30" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B30" s="46"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="49"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="67"/>
       <c r="F30" s="49"/>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="35"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="68"/>
       <c r="K30" s="35"/>
       <c r="L30" s="35"/>
-    </row>
-    <row r="31" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M30" s="35"/>
+    </row>
+    <row r="31" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="49"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="49"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="35"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="68"/>
       <c r="K31" s="35"/>
       <c r="L31" s="35"/>
-    </row>
-    <row r="32" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M31" s="35"/>
+    </row>
+    <row r="32" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="49"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="67"/>
       <c r="F32" s="49"/>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="35"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="68"/>
       <c r="K32" s="35"/>
       <c r="L32" s="35"/>
-    </row>
-    <row r="33" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M32" s="35"/>
+    </row>
+    <row r="33" spans="2:13" ht="16" x14ac:dyDescent="0.4">
       <c r="B33" s="46"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="49"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="49"/>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="35"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="68"/>
       <c r="K33" s="35"/>
       <c r="L33" s="35"/>
-    </row>
-    <row r="34" spans="2:12" ht="16" x14ac:dyDescent="0.4">
+      <c r="M33" s="35"/>
+    </row>
+    <row r="34" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B34" s="59"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="70"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="35"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="71"/>
       <c r="K34" s="35"/>
       <c r="L34" s="35"/>
-    </row>
-    <row r="35" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="M34" s="35"/>
+    </row>
+    <row r="35" spans="2:13" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="35"/>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="35"/>
+      <c r="D35" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="60">
+      <c r="E35" s="60">
         <v>3</v>
       </c>
-      <c r="E35" s="60">
+      <c r="F35" s="60">
         <v>1</v>
       </c>
-      <c r="F35" s="60">
+      <c r="G35" s="60">
         <v>0</v>
-      </c>
-      <c r="G35" s="60">
-        <v>3</v>
       </c>
       <c r="H35" s="60">
         <v>3</v>
       </c>
       <c r="I35" s="60">
+        <v>3</v>
+      </c>
+      <c r="J35" s="60">
         <v>1</v>
       </c>
-      <c r="J35" s="35"/>
       <c r="K35" s="35"/>
       <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="L9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3325,6 +3403,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1eec4c4c-619d-4796-91a6-89c807311e80">
@@ -3333,15 +3420,6 @@
     <TaxCatchAll xmlns="7ad6aa05-2b5c-4683-81b2-fe78918efd15" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3364,6 +3442,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA4C34A-1173-435D-BDBC-FEA8FF547DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75092B96-EF1C-4949-8CF0-BA6FA8CE960D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3372,12 +3458,4 @@
     <ds:schemaRef ds:uri="7ad6aa05-2b5c-4683-81b2-fe78918efd15"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA4C34A-1173-435D-BDBC-FEA8FF547DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finished readPrefFolder, fixed bugs in readStatusInfo
</commit_message>
<xml_diff>
--- a/Example_Data/TripsAndLeaderStatusInfo.xlsx
+++ b/Example_Data/TripsAndLeaderStatusInfo.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shume\Documents\Example Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9F841A-221D-408C-995B-5D7FEDE172BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D5C963-47DE-4F5F-859B-43C01E015FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="23980" windowHeight="15280" activeTab="1" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="23980" windowHeight="15280" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prefs Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Trip Info" sheetId="1" r:id="rId1"/>
     <sheet name="Trip Leader Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -1388,31 +1388,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56457AC2-4CCE-48AB-B957-6565BDA2DBE4}">
-  <dimension ref="B2:J59"/>
+  <dimension ref="B1:H59"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="68.1796875" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
     <col min="5" max="5" width="31.26953125" customWidth="1"/>
     <col min="6" max="6" width="35.453125" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>3</v>
@@ -1424,15 +1425,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="31">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="31">
         <v>45318</v>
       </c>
-      <c r="C3" s="31">
+      <c r="D3" s="31">
         <v>45319</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>7</v>
@@ -1444,23 +1445,15 @@
         <f>IF(F3=2, 1, 2)</f>
         <v>2</v>
       </c>
-      <c r="H3" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1, 6), "Overnight", "Biking","Spelunking", "Watersports", "Surfing", "Sea Kayaking")</f>
-        <v>Overnight</v>
-      </c>
-      <c r="J3">
-        <f ca="1">CHOOSE(RANDBETWEEN(1, 2), 2, 4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="7">
+    </row>
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7">
         <v>45318</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1472,14 +1465,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="9">
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
         <v>45319</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1491,14 +1484,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="11">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11">
         <v>45322</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="D6" s="11"/>
       <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1510,15 +1503,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="31">
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="31">
         <v>45324</v>
       </c>
-      <c r="C7" s="31">
+      <c r="D7" s="31">
         <v>45326</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>13</v>
@@ -1531,15 +1524,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="24">
+    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24">
         <v>45331</v>
       </c>
-      <c r="C8" s="24">
+      <c r="D8" s="24">
         <v>45333</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>11</v>
@@ -1552,14 +1545,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="14">
+    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14">
         <v>45332</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
-        <v>16</v>
-      </c>
+      <c r="D9" s="14"/>
       <c r="E9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1571,14 +1564,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="14">
+    <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14">
         <v>45332</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="D10" s="14"/>
       <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1590,14 +1583,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="14">
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14">
         <v>45333</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1609,14 +1602,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="9">
+    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="9">
         <v>45333</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1628,14 +1621,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="16">
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16">
         <v>45336</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="D13" s="16"/>
       <c r="E13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1647,14 +1640,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="14">
+    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="14">
         <v>45339</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="D14" s="14"/>
       <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
@@ -1666,14 +1659,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="18">
+    <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="18">
         <v>45339</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19" t="s">
-        <v>24</v>
-      </c>
+      <c r="D15" s="18"/>
       <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1685,14 +1678,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="14">
+    <row r="16" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="14">
         <v>45340</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="D16" s="14"/>
       <c r="E16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1705,13 +1698,13 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="9">
+      <c r="B17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9">
         <v>45340</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1725,13 +1718,13 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="20">
+      <c r="B18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="20">
         <v>45343</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="D18" s="20"/>
       <c r="E18" s="5" t="s">
         <v>13</v>
       </c>
@@ -1745,13 +1738,13 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="7">
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="7">
         <v>45344</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="D19" s="7"/>
       <c r="E19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1765,14 +1758,14 @@
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="7">
+      <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7">
         <v>45346</v>
       </c>
-      <c r="C20" s="7">
+      <c r="D20" s="7">
         <v>45347</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>17</v>
@@ -1786,13 +1779,13 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="7">
+      <c r="B21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7">
         <v>45346</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
@@ -1805,13 +1798,13 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="7">
+      <c r="B22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="7">
         <v>45346</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1824,13 +1817,13 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="11">
+      <c r="B23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="11">
         <v>45347</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="D23" s="11"/>
       <c r="E23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1843,14 +1836,14 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="16">
+      <c r="B24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="16">
         <v>45352</v>
       </c>
-      <c r="C24" s="16">
+      <c r="D24" s="16">
         <v>45354</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>11</v>
@@ -1864,14 +1857,14 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="16">
+      <c r="B25" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="16">
         <v>45353</v>
       </c>
-      <c r="C25" s="16">
+      <c r="D25" s="16">
         <v>45354</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
@@ -1885,13 +1878,13 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="14">
+      <c r="B26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="14">
         <v>45353</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15" t="s">
-        <v>35</v>
-      </c>
+      <c r="D26" s="14"/>
       <c r="E26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1904,13 +1897,13 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="18">
+      <c r="B27" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="18">
         <v>45354</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="D27" s="18"/>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1923,14 +1916,14 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="24">
+      <c r="B28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="24">
         <v>45359</v>
       </c>
-      <c r="C28" s="24">
+      <c r="D28" s="24">
         <v>45361</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>11</v>
@@ -1944,14 +1937,14 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="16">
+      <c r="B29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="16">
         <v>45360</v>
       </c>
-      <c r="C29" s="16">
+      <c r="D29" s="16">
         <v>45368</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>9</v>
@@ -1965,14 +1958,14 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="16">
+      <c r="B30" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="16">
         <v>45360</v>
       </c>
-      <c r="C30" s="14">
+      <c r="D30" s="14">
         <v>45364</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>21</v>
@@ -1986,14 +1979,14 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="14">
+      <c r="B31" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="14">
         <v>45361</v>
       </c>
-      <c r="C31" s="14">
+      <c r="D31" s="14">
         <v>45365</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>9</v>
@@ -2007,13 +2000,13 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="16">
+      <c r="B32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="16">
         <v>45371</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="17" t="s">
-        <v>41</v>
-      </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="5" t="s">
         <v>11</v>
       </c>
@@ -2026,14 +2019,14 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="14">
+      <c r="B33" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14">
         <v>45361</v>
       </c>
-      <c r="C33" s="9">
+      <c r="D33" s="9">
         <v>45365</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>17</v>
@@ -2047,13 +2040,13 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="18">
+      <c r="B34" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="18">
         <v>45374</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="D34" s="18"/>
       <c r="E34" s="5" t="s">
         <v>21</v>
       </c>
@@ -2066,13 +2059,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="14">
+      <c r="B35" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="14">
         <v>45374</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="D35" s="14"/>
       <c r="E35" s="5" t="s">
         <v>7</v>
       </c>
@@ -2085,13 +2078,13 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="14">
+      <c r="B36" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="14">
         <v>45375</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="D36" s="14"/>
       <c r="E36" s="5" t="s">
         <v>9</v>
       </c>
@@ -2104,13 +2097,13 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="9">
+      <c r="B37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="9">
         <v>45375</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="D37" s="9"/>
       <c r="E37" s="5" t="s">
         <v>11</v>
       </c>
@@ -2123,14 +2116,14 @@
       </c>
     </row>
     <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="20">
+      <c r="B38" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="20">
         <v>45380</v>
       </c>
-      <c r="C38" s="20">
+      <c r="D38" s="20">
         <v>45382</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>17</v>
@@ -2144,14 +2137,14 @@
       </c>
     </row>
     <row r="39" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="32">
+      <c r="B39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="32">
         <v>45381</v>
       </c>
-      <c r="C39" s="32">
+      <c r="D39" s="32">
         <v>45382</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>17</v>
@@ -2165,13 +2158,13 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="7">
+      <c r="B40" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="7">
         <v>45381</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
         <v>7</v>
       </c>
@@ -2184,13 +2177,13 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="22">
+      <c r="B41" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="22">
         <v>45382</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="D41" s="22"/>
       <c r="E41" s="5" t="s">
         <v>13</v>
       </c>
@@ -2203,13 +2196,13 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="24">
+      <c r="B42" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="24">
         <v>45384</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="D42" s="24"/>
       <c r="E42" s="5" t="s">
         <v>7</v>
       </c>
@@ -2222,14 +2215,14 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="14">
+      <c r="B43" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="14">
         <v>45387</v>
       </c>
-      <c r="C43" s="14">
+      <c r="D43" s="14">
         <v>45389</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>9</v>
@@ -2243,13 +2236,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="14">
+      <c r="B44" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="14">
         <v>45388</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="D44" s="14"/>
       <c r="E44" s="5" t="s">
         <v>9</v>
       </c>
@@ -2262,13 +2255,13 @@
       </c>
     </row>
     <row r="45" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="14">
+      <c r="B45" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="14">
         <v>45389</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="D45" s="14"/>
       <c r="E45" s="5" t="s">
         <v>7</v>
       </c>
@@ -2281,14 +2274,14 @@
       </c>
     </row>
     <row r="46" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="24">
+      <c r="B46" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="24">
         <v>45394</v>
       </c>
-      <c r="C46" s="24">
+      <c r="D46" s="24">
         <v>45396</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>9</v>
@@ -2302,14 +2295,14 @@
       </c>
     </row>
     <row r="47" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="14">
+      <c r="B47" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="14">
         <v>45394</v>
       </c>
-      <c r="C47" s="14">
+      <c r="D47" s="14">
         <v>45396</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>13</v>
@@ -2323,13 +2316,13 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="18">
+      <c r="B48" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="18">
         <v>45395</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19" t="s">
-        <v>57</v>
-      </c>
+      <c r="D48" s="18"/>
       <c r="E48" s="5" t="s">
         <v>7</v>
       </c>
@@ -2342,13 +2335,13 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="18">
+      <c r="B49" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="18">
         <v>45396</v>
       </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19" t="s">
-        <v>58</v>
-      </c>
+      <c r="D49" s="18"/>
       <c r="E49" s="5" t="s">
         <v>17</v>
       </c>
@@ -2361,14 +2354,14 @@
       </c>
     </row>
     <row r="50" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="24">
+      <c r="B50" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="24">
         <v>45401</v>
       </c>
-      <c r="C50" s="24">
+      <c r="D50" s="24">
         <v>45403</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>13</v>
@@ -2382,14 +2375,14 @@
       </c>
     </row>
     <row r="51" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="24">
+      <c r="B51" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="24">
         <v>45401</v>
       </c>
-      <c r="C51" s="24">
+      <c r="D51" s="24">
         <v>45403</v>
-      </c>
-      <c r="D51" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>13</v>
@@ -2403,14 +2396,14 @@
       </c>
     </row>
     <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="24">
+      <c r="B52" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="24">
         <v>45401</v>
       </c>
-      <c r="C52" s="24">
+      <c r="D52" s="24">
         <v>45403</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>61</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>13</v>
@@ -2424,14 +2417,14 @@
       </c>
     </row>
     <row r="53" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="31">
+      <c r="B53" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="31">
         <v>45408</v>
       </c>
-      <c r="C53" s="31">
+      <c r="D53" s="31">
         <v>45410</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>17</v>
@@ -2445,14 +2438,14 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="31">
+      <c r="B54" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="31">
         <v>45408</v>
       </c>
-      <c r="C54" s="31">
+      <c r="D54" s="31">
         <v>45410</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>17</v>
@@ -2466,13 +2459,13 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="11">
+      <c r="B55" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="11">
         <v>45410</v>
       </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="D55" s="11"/>
       <c r="E55" s="5" t="s">
         <v>9</v>
       </c>
@@ -2485,13 +2478,13 @@
       </c>
     </row>
     <row r="56" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="11">
+      <c r="B56" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="11">
         <v>45408</v>
       </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="D56" s="28"/>
       <c r="E56" s="5" t="s">
         <v>13</v>
       </c>
@@ -2504,14 +2497,14 @@
       </c>
     </row>
     <row r="57" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="33">
+      <c r="B57" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="33">
         <v>45417</v>
       </c>
-      <c r="C57" s="33">
+      <c r="D57" s="33">
         <v>45423</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>17</v>
@@ -2525,14 +2518,14 @@
       </c>
     </row>
     <row r="58" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="34">
+      <c r="B58" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="34">
         <v>45417</v>
       </c>
-      <c r="C58" s="34">
+      <c r="D58" s="34">
         <v>45420</v>
-      </c>
-      <c r="D58" s="30" t="s">
-        <v>67</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>13</v>
@@ -2546,14 +2539,14 @@
       </c>
     </row>
     <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="34">
+      <c r="B59" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="34">
         <v>45514</v>
       </c>
-      <c r="C59" s="34">
+      <c r="D59" s="34">
         <v>45523</v>
-      </c>
-      <c r="D59" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>7</v>
@@ -2586,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445B6131-D158-4A66-8748-C0EBB6C75469}">
   <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>